<commit_message>
update and Add Binary
</commit_message>
<xml_diff>
--- a/MyHints.xlsx
+++ b/MyHints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psol/Documents/ProblemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF02DD2A-40A2-DE44-AD06-976E9B523D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EE48E2-CE83-DF43-A807-DDB9E755734E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{F8E361A5-22B9-4240-8BC8-52C1D347E6C7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>PROBLEM</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>break string into array. Push all into stack. popLast for string value &gt;= 1</t>
+  </si>
+  <si>
+    <t>Plus One</t>
+  </si>
+  <si>
+    <t>Plus One( Adding 1 to large intDo not attempt to convert from dtring to Int. Instead use for loop from behind/reversed, and for every count in the for loop, use a while loop to pop the last item and add 1. maintain condition if sum &gt; 9</t>
   </si>
 </sst>
 </file>
@@ -481,9 +487,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE287B7-E7B1-A34A-B32A-2EBD5518F426}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -579,6 +585,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="68">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>